<commit_message>
add ftsemib to ticker list
</commit_message>
<xml_diff>
--- a/data/ticker/it/ticker.xlsx
+++ b/data/ticker/it/ticker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l_ace\Desktop\projects\algoshort_other\data\ticker\it\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l_ace\Desktop\projects\myfinance2\data\ticker\it\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{935907F9-A399-477E-837A-11B79D52E786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706DC571-F510-4B02-9515-AC110E9F300F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{01610EC7-D974-46FE-AB54-375AC97826ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="607">
   <si>
     <t>name</t>
   </si>
@@ -1854,6 +1854,9 @@
   </si>
   <si>
     <t>PRT.MI</t>
+  </si>
+  <si>
+    <t>FTSEMIB.IT</t>
   </si>
 </sst>
 </file>
@@ -2225,9 +2228,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D2F36A-15C4-452F-9225-8648A1292D43}">
-  <dimension ref="A1:B305"/>
+  <dimension ref="A1:B306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="B307" sqref="B307"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -4671,6 +4676,11 @@
         <v>605</v>
       </c>
     </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B306" t="s">
+        <v>606</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>